<commit_message>
Add default value for keterangan in import_ajax and update Excel template
</commit_message>
<xml_diff>
--- a/PBLSEM4/public/template_mahasiswa.xlsx
+++ b/PBLSEM4/public/template_mahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SIPINTA\PBLSEM4\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AE3B4-E16A-4BF5-8877-E07DF36E45F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1524D4EF-3640-41CD-8889-1395FCCDA8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>nim</t>
   </si>
@@ -60,15 +60,9 @@
     <t>aktif</t>
   </si>
   <si>
-    <t>Aprilia Putri</t>
-  </si>
-  <si>
     <t>no_telp</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3514226204050008</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 085755742091</t>
   </si>
   <si>
@@ -78,16 +72,13 @@
     <t>alamat_sekarang</t>
   </si>
   <si>
-    <t>Pasuruan</t>
-  </si>
-  <si>
     <t>Malang</t>
   </si>
   <si>
-    <t>keterangan</t>
-  </si>
-  <si>
-    <t>gratis</t>
+    <t>Indi Warda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3507166210050002</t>
   </si>
 </sst>
 </file>
@@ -620,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.26953125" defaultRowHeight="14.5"/>
@@ -635,7 +626,7 @@
     <col min="6" max="7" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,13 +640,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -664,33 +655,30 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2">
-        <v>2341760043</v>
+        <v>2341760026</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>2023</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -698,23 +686,20 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2">
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:10">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="B6" s="1"/>
     </row>
   </sheetData>

</xml_diff>